<commit_message>
ITSADSSD-20677 - IAA_IELTS  SI-net navigation and find IELTS
Add navigation to Maintain Application and UQ Qualification Data and unit testing
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -333,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -343,6 +343,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -363,15 +369,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,7 +662,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -757,7 +766,7 @@
       <c r="A7" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
@@ -1953,6 +1962,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ITSADSSD-20956 - Take IELTS result screenshot and upload in SI-net
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -373,10 +373,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -662,7 +661,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -766,7 +765,7 @@
       <c r="A7" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C7" t="s">
@@ -1963,6 +1962,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ITSADSSD-21274 - IELTS - Verify Test Components Score
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -230,9 +230,6 @@
     <t>exceptionEmailAddress_DEV</t>
   </si>
   <si>
-    <t>bpm.ads@its.uq.edu.au</t>
-  </si>
-  <si>
     <t>Email address to send application exception emails to DEV environment</t>
   </si>
   <si>
@@ -281,52 +278,82 @@
     <t>smtp port number (MUST BE AN INTEGER)</t>
   </si>
   <si>
-    <t>allowedItemList</t>
-  </si>
-  <si>
-    <t>CONFIR,EXTCON,MIDREV,EXTMID,THEREV,EXTTHE,SUBMDL,EXTSUB</t>
-  </si>
-  <si>
-    <t>List of allowed Item codes</t>
+    <t>https://sa92fnta.dev.sinet.uq.edu.au</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>mySI_netApplicationDocumentsSearch_DEV</t>
+  </si>
+  <si>
+    <t>mySI_netApplicationDocumentsSearch_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netApplicationDocumentsSearch_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netApplicationDocumentsSearch_PROD</t>
+  </si>
+  <si>
+    <t>mySI_netMaintainApplicationsSearch_DEV</t>
+  </si>
+  <si>
+    <t>mySI_netMaintainApplicationsSearch_TEST</t>
+  </si>
+  <si>
+    <t>mySI_netMaintainApplicationsSearch_STAGING</t>
+  </si>
+  <si>
+    <t>mySI_netMaintainApplicationsSearch_PROD</t>
+  </si>
+  <si>
+    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
+  </si>
+  <si>
+    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
+  </si>
+  <si>
+    <t>IAA_IELTS_Sample_Queue</t>
+  </si>
+  <si>
+    <t>SSO_rpaapl01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ Single Sign On account for Ivy </t>
+  </si>
+  <si>
+    <t>IAA_IELTS_Account</t>
+  </si>
+  <si>
+    <t>IAA_IELTS_SPOKED_DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy login credentails for IELTS website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credentails to connect with database </t>
+  </si>
+  <si>
+    <t>rpa.ads@its.uq.edu.au</t>
+  </si>
+  <si>
+    <t>BusinessProcessName</t>
   </si>
   <si>
     <t>IAA_IELTS</t>
   </si>
   <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>mySI_netApplicationDocumentsSearch_DEV</t>
-  </si>
-  <si>
-    <t>mySI_netApplicationDocumentsSearch_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netApplicationDocumentsSearch_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netApplicationDocumentsSearch_PROD</t>
-  </si>
-  <si>
-    <t>mySI_netMaintainApplicationsSearch_DEV</t>
-  </si>
-  <si>
-    <t>mySI_netMaintainApplicationsSearch_TEST</t>
-  </si>
-  <si>
-    <t>mySI_netMaintainApplicationsSearch_STAGING</t>
-  </si>
-  <si>
-    <t>mySI_netMaintainApplicationsSearch_PROD</t>
-  </si>
-  <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
-  </si>
-  <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
+    <t>Business Process Name</t>
+  </si>
+  <si>
+    <t>IELTS_URL</t>
+  </si>
+  <si>
+    <t>https://ielts.ucles.org.uk/ielts-trf/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IELTS website login page </t>
   </si>
 </sst>
 </file>
@@ -373,10 +400,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -661,7 +689,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -711,7 +739,7 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -722,7 +750,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -733,7 +761,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -744,7 +772,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -763,10 +791,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -774,10 +802,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>55</v>
@@ -785,10 +813,10 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
@@ -796,10 +824,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
@@ -807,10 +835,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -818,10 +846,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>55</v>
@@ -829,10 +857,10 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>56</v>
@@ -840,10 +868,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
@@ -894,108 +922,108 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>587</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-    </row>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1963,6 +1991,9 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
     <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B23" r:id="rId4"/>
+    <hyperlink ref="B24:B26" r:id="rId5" display="rpa.ads@its.uq.edu.au"/>
+    <hyperlink ref="B20" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1972,7 +2003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2016,7 +2049,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
@@ -3184,7 +3227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3225,9 +3270,39 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-21501 - SInet / IELTS logout changes
SInet / IELTS logout changes, amendment in Login and extract SInet details
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t xml:space="preserve">IELTS website login page </t>
+  </si>
+  <si>
+    <t>IELTSResult_Screenshot</t>
+  </si>
+  <si>
+    <t>IELTSResultScreenshotFolder</t>
+  </si>
+  <si>
+    <t>Where to save IELTS result screenshots - a relative path.</t>
   </si>
 </sst>
 </file>
@@ -689,7 +698,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2001,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2114,134 +2123,144 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>15000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>60000</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>0.8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>0.9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3218,6 +3237,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ITSADSSD-23537 - Code clean up, add email template and config update
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -89,24 +89,6 @@
     <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
   </si>
   <si>
-    <t>AccuracyLow</t>
-  </si>
-  <si>
-    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyMedium</t>
-  </si>
-  <si>
-    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyHigh</t>
-  </si>
-  <si>
-    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
@@ -251,36 +233,6 @@
     <t>Email address to send application exception emails to PROD environment</t>
   </si>
   <si>
-    <t>partTimeExtension</t>
-  </si>
-  <si>
-    <t>How many months to extend for part time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>fullTimeExtension</t>
-  </si>
-  <si>
-    <t>How many months to extend for full time students (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>smtpServer</t>
-  </si>
-  <si>
-    <t>smtp.uq.edu.au</t>
-  </si>
-  <si>
-    <t>smtp server to use to send emails</t>
-  </si>
-  <si>
-    <t>smtpPort</t>
-  </si>
-  <si>
-    <t>smtp port number (MUST BE AN INTEGER)</t>
-  </si>
-  <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au</t>
-  </si>
-  <si>
     <t>TBC</t>
   </si>
   <si>
@@ -308,15 +260,6 @@
     <t>mySI_netMaintainApplicationsSearch_PROD</t>
   </si>
   <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
-  </si>
-  <si>
-    <t>https://sa92fnta.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
-  </si>
-  <si>
-    <t>IAA_IELTS_Sample_Queue</t>
-  </si>
-  <si>
     <t>SSO_rpaapl01</t>
   </si>
   <si>
@@ -363,13 +306,139 @@
   </si>
   <si>
     <t>Where to save IELTS result screenshots - a relative path.</t>
+  </si>
+  <si>
+    <t>manish.gupta@uq.edu.au</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au</t>
+  </si>
+  <si>
+    <t>cloud-cmgw.compute.dc.uq.edu.au</t>
+  </si>
+  <si>
+    <t>Oracle database hostname used to connect robot to database when running from DEV, TEST, STAGING or PROD</t>
+  </si>
+  <si>
+    <t>Oracle database hostname used to connect robot to database when running through local machine</t>
+  </si>
+  <si>
+    <t>conman1.compute.dc.uq.edu.au</t>
+  </si>
+  <si>
+    <t>DB_Cloud_Hostname</t>
+  </si>
+  <si>
+    <t>DB_ServiceName</t>
+  </si>
+  <si>
+    <t>SPOKED.SOE.UQ.EDU.AU</t>
+  </si>
+  <si>
+    <t>Oracle database service name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle database port number </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>UQ internal SMTP Server</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ internal SMTP Server Port number </t>
+  </si>
+  <si>
+    <t>PROD_Subject</t>
+  </si>
+  <si>
+    <t>NonPROD_Subject</t>
+  </si>
+  <si>
+    <t>Ivy found error(s) while processing</t>
+  </si>
+  <si>
+    <t>Ivy {0} found error(s) while processing</t>
+  </si>
+  <si>
+    <t>IvyErrorEmailMsg</t>
+  </si>
+  <si>
+    <t>You are receiving this email from the RPA robot due to an error encountered during the IAA_IELTS process. Error message {0}. Please see attached screenshot.</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName_NP</t>
+  </si>
+  <si>
+    <t>SenderEmailID</t>
+  </si>
+  <si>
+    <t>noreply@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Ivy - RPA Bot</t>
+  </si>
+  <si>
+    <t>Ivy {0} - RPA Bot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy bot display name for email notifications </t>
+  </si>
+  <si>
+    <t>Ivy bot display name for email notifications for Non Prod environments (Dev/Test/Staging)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy bot sender email (for display purpose) email sent through SMTP </t>
+  </si>
+  <si>
+    <t>DocumentDescription</t>
+  </si>
+  <si>
+    <t>IELTS Test Result</t>
+  </si>
+  <si>
+    <t>MaxQueueItem</t>
+  </si>
+  <si>
+    <t>IAA_IELTS_MaxOueueItem</t>
+  </si>
+  <si>
+    <t>Orchestrator asset hold integer value which control number of records fetch from database, serve as ROWNUM in sql query</t>
+  </si>
+  <si>
+    <t>DB_PortNumber</t>
+  </si>
+  <si>
+    <t>Document description for UQ Application Document upload</t>
+  </si>
+  <si>
+    <t>Subject for error notification in PROD environment</t>
+  </si>
+  <si>
+    <t>Subject for error notification in Non-PROD environment</t>
+  </si>
+  <si>
+    <t>Email message body for error notification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -386,6 +455,12 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,11 +484,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,7 +777,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,293 +824,253 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>86</v>
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" t="s">
-        <v>86</v>
+        <v>72</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" t="s">
-        <v>86</v>
+        <v>73</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30">
-        <v>587</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
-      </c>
-    </row>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2003,6 +2042,9 @@
     <hyperlink ref="B23" r:id="rId4"/>
     <hyperlink ref="B24:B26" r:id="rId5" display="rpa.ads@its.uq.edu.au"/>
     <hyperlink ref="B20" r:id="rId6"/>
+    <hyperlink ref="B4:B5" r:id="rId7" display="https://sa92prep.dev.sinet.uq.edu.au"/>
+    <hyperlink ref="B8:B9" r:id="rId8" display="https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL"/>
+    <hyperlink ref="B12:B13" r:id="rId9" display="https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2010,17 +2052,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="3" max="3" width="102.5703125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2060,13 +2102,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2123,15 +2165,15 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -2176,115 +2218,205 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
-        <v>0.6</v>
+      <c r="B16" t="s">
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>0.8</v>
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18">
-        <v>0.9</v>
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-    </row>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1521</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3234,11 +3366,10 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B35" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3248,7 +3379,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3292,39 +3423,59 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-23380 - Change for TakeScreenshot activity and amend config
'IELTS_Screenshot' folder not pick by Jenkins as being an empty folder. Using TakeScreenshot.xaml to check  folder exists, if not create it.
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>Email message body for error notification</t>
+  </si>
+  <si>
+    <t>DB_Local_Hostname</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2054,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2283,7 +2286,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B23" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
ITSADSSD-23512 - Changes in config and ExtractTRF Result
</commit_message>
<xml_diff>
--- a/Processes/IAA_IELTS/Data/Config.xlsx
+++ b/Processes/IAA_IELTS/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -293,148 +293,148 @@
     <t>IELTS_URL</t>
   </si>
   <si>
+    <t xml:space="preserve">IELTS website login page </t>
+  </si>
+  <si>
+    <t>IELTSResult_Screenshot</t>
+  </si>
+  <si>
+    <t>IELTSResultScreenshotFolder</t>
+  </si>
+  <si>
+    <t>Where to save IELTS result screenshots - a relative path.</t>
+  </si>
+  <si>
+    <t>manish.gupta@uq.edu.au</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
+  </si>
+  <si>
+    <t>https://sa92prep.dev.sinet.uq.edu.au</t>
+  </si>
+  <si>
+    <t>cloud-cmgw.compute.dc.uq.edu.au</t>
+  </si>
+  <si>
+    <t>Oracle database hostname used to connect robot to database when running from DEV, TEST, STAGING or PROD</t>
+  </si>
+  <si>
+    <t>Oracle database hostname used to connect robot to database when running through local machine</t>
+  </si>
+  <si>
+    <t>conman1.compute.dc.uq.edu.au</t>
+  </si>
+  <si>
+    <t>DB_Cloud_Hostname</t>
+  </si>
+  <si>
+    <t>DB_ServiceName</t>
+  </si>
+  <si>
+    <t>SPOKED.SOE.UQ.EDU.AU</t>
+  </si>
+  <si>
+    <t>Oracle database service name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle database port number </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>UQ internal SMTP Server</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ internal SMTP Server Port number </t>
+  </si>
+  <si>
+    <t>PROD_Subject</t>
+  </si>
+  <si>
+    <t>NonPROD_Subject</t>
+  </si>
+  <si>
+    <t>Ivy found error(s) while processing</t>
+  </si>
+  <si>
+    <t>Ivy {0} found error(s) while processing</t>
+  </si>
+  <si>
+    <t>IvyErrorEmailMsg</t>
+  </si>
+  <si>
+    <t>You are receiving this email from the RPA robot due to an error encountered during the IAA_IELTS process. Error message {0}. Please see attached screenshot.</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName</t>
+  </si>
+  <si>
+    <t>EmailSenderDisplayName_NP</t>
+  </si>
+  <si>
+    <t>SenderEmailID</t>
+  </si>
+  <si>
+    <t>noreply@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Ivy - RPA Bot</t>
+  </si>
+  <si>
+    <t>Ivy {0} - RPA Bot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy bot display name for email notifications </t>
+  </si>
+  <si>
+    <t>Ivy bot display name for email notifications for Non Prod environments (Dev/Test/Staging)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivy bot sender email (for display purpose) email sent through SMTP </t>
+  </si>
+  <si>
+    <t>DocumentDescription</t>
+  </si>
+  <si>
+    <t>IELTS Test Result</t>
+  </si>
+  <si>
+    <t>MaxQueueItem</t>
+  </si>
+  <si>
+    <t>IAA_IELTS_MaxOueueItem</t>
+  </si>
+  <si>
+    <t>Orchestrator asset hold integer value which control number of records fetch from database, serve as ROWNUM in sql query</t>
+  </si>
+  <si>
+    <t>DB_PortNumber</t>
+  </si>
+  <si>
+    <t>Document description for UQ Application Document upload</t>
+  </si>
+  <si>
+    <t>Subject for error notification in PROD environment</t>
+  </si>
+  <si>
+    <t>Subject for error notification in Non-PROD environment</t>
+  </si>
+  <si>
+    <t>Email message body for error notification</t>
+  </si>
+  <si>
+    <t>DB_Local_Hostname</t>
+  </si>
+  <si>
     <t>https://ielts.ucles.org.uk/ielts-trf/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IELTS website login page </t>
-  </si>
-  <si>
-    <t>IELTSResult_Screenshot</t>
-  </si>
-  <si>
-    <t>IELTSResultScreenshotFolder</t>
-  </si>
-  <si>
-    <t>Where to save IELTS result screenshots - a relative path.</t>
-  </si>
-  <si>
-    <t>manish.gupta@uq.edu.au</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/PROCESS_APPLICATIONS.ADM_APPL_MAINTNCE.GBL</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au/psp/ps/EMPLOYEE/SA/c/UQ_AD1_MENU.UQ_APPL_EVIDENCE.GBL</t>
-  </si>
-  <si>
-    <t>https://sa92prep.dev.sinet.uq.edu.au</t>
-  </si>
-  <si>
-    <t>cloud-cmgw.compute.dc.uq.edu.au</t>
-  </si>
-  <si>
-    <t>Oracle database hostname used to connect robot to database when running from DEV, TEST, STAGING or PROD</t>
-  </si>
-  <si>
-    <t>Oracle database hostname used to connect robot to database when running through local machine</t>
-  </si>
-  <si>
-    <t>conman1.compute.dc.uq.edu.au</t>
-  </si>
-  <si>
-    <t>DB_Cloud_Hostname</t>
-  </si>
-  <si>
-    <t>DB_ServiceName</t>
-  </si>
-  <si>
-    <t>SPOKED.SOE.UQ.EDU.AU</t>
-  </si>
-  <si>
-    <t>Oracle database service name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle database port number </t>
-  </si>
-  <si>
-    <t>UQ_SMTP_SERVER</t>
-  </si>
-  <si>
-    <t>UQ internal SMTP Server</t>
-  </si>
-  <si>
-    <t>UQ_SMTP_PORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UQ internal SMTP Server Port number </t>
-  </si>
-  <si>
-    <t>PROD_Subject</t>
-  </si>
-  <si>
-    <t>NonPROD_Subject</t>
-  </si>
-  <si>
-    <t>Ivy found error(s) while processing</t>
-  </si>
-  <si>
-    <t>Ivy {0} found error(s) while processing</t>
-  </si>
-  <si>
-    <t>IvyErrorEmailMsg</t>
-  </si>
-  <si>
-    <t>You are receiving this email from the RPA robot due to an error encountered during the IAA_IELTS process. Error message {0}. Please see attached screenshot.</t>
-  </si>
-  <si>
-    <t>EmailSenderDisplayName</t>
-  </si>
-  <si>
-    <t>EmailSenderDisplayName_NP</t>
-  </si>
-  <si>
-    <t>SenderEmailID</t>
-  </si>
-  <si>
-    <t>noreply@uq.edu.au</t>
-  </si>
-  <si>
-    <t>Ivy - RPA Bot</t>
-  </si>
-  <si>
-    <t>Ivy {0} - RPA Bot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivy bot display name for email notifications </t>
-  </si>
-  <si>
-    <t>Ivy bot display name for email notifications for Non Prod environments (Dev/Test/Staging)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivy bot sender email (for display purpose) email sent through SMTP </t>
-  </si>
-  <si>
-    <t>DocumentDescription</t>
-  </si>
-  <si>
-    <t>IELTS Test Result</t>
-  </si>
-  <si>
-    <t>MaxQueueItem</t>
-  </si>
-  <si>
-    <t>IAA_IELTS_MaxOueueItem</t>
-  </si>
-  <si>
-    <t>Orchestrator asset hold integer value which control number of records fetch from database, serve as ROWNUM in sql query</t>
-  </si>
-  <si>
-    <t>DB_PortNumber</t>
-  </si>
-  <si>
-    <t>Document description for UQ Application Document upload</t>
-  </si>
-  <si>
-    <t>Subject for error notification in PROD environment</t>
-  </si>
-  <si>
-    <t>Subject for error notification in Non-PROD environment</t>
-  </si>
-  <si>
-    <t>Email message body for error notification</t>
-  </si>
-  <si>
-    <t>DB_Local_Hostname</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -841,7 +841,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -852,7 +852,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>42</v>
@@ -863,7 +863,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -885,7 +885,7 @@
         <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
@@ -896,7 +896,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>49</v>
@@ -907,7 +907,7 @@
         <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
@@ -929,7 +929,7 @@
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
@@ -940,7 +940,7 @@
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -951,7 +951,7 @@
         <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -1018,10 +1018,10 @@
         <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" t="s">
         <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1031,7 @@
         <v>62</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>63</v>
@@ -2057,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2168,15 +2168,15 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -2275,136 +2275,136 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
         <v>104</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>105</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="4">
         <v>1521</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
         <v>127</v>
       </c>
-      <c r="B27" t="s">
-        <v>128</v>
-      </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" t="s">
         <v>129</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>130</v>
-      </c>
-      <c r="C30" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3459,24 +3459,24 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>